<commit_message>
Se crea aplicación para unir archivos
Se crea aplicación unions que une y clasifica en hábil y no hábil los
resultados.
</commit_message>
<xml_diff>
--- a/archives/in/PE/CANT_SCP_PROF_PM25.xlsx
+++ b/archives/in/PE/CANT_SCP_PROF_PM25.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\ULS-ECP-SDA\Entregables\5. Quinto_Entregable\Speciation_PM25_per_source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\ULS-ECP-SDA\Entregables\5. Quinto_Entregable\Others\Speciation_per_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="CANT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>PM2_5</t>
   </si>
@@ -32,9 +32,6 @@
     <t>POC</t>
   </si>
   <si>
-    <t>PNH4</t>
-  </si>
-  <si>
     <t>PNO3</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>PSI</t>
   </si>
   <si>
-    <t>PCL</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
   </si>
   <si>
     <t>PFE</t>
-  </si>
-  <si>
-    <t>PMOTHR</t>
   </si>
   <si>
     <t>SOURCE</t>
@@ -213,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -248,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -433,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,30 +437,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2">
         <v>92022</v>
@@ -477,22 +468,22 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>5.3800000000000001E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>5.3800000000000001E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>92022</v>
@@ -500,22 +491,22 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="3">
-        <v>2.0500000000000002E-3</v>
+        <v>1.47E-2</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="3">
-        <v>2.0500000000000002E-3</v>
+        <v>1.47E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2">
         <v>92022</v>
@@ -523,22 +514,22 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>1.25E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <v>1.25E-3</v>
+        <v>2.7100000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
         <v>92022</v>
@@ -546,22 +537,22 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3">
-        <v>5.8799999999999998E-4</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="3">
-        <v>5.8799999999999998E-4</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>92022</v>
@@ -569,22 +560,22 @@
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="2">
-        <v>1.8E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>1.8E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>92022</v>
@@ -592,22 +583,22 @@
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>2.1499999999999998E-2</v>
+        <v>3.3700000000000001E-2</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>2.1499999999999998E-2</v>
+        <v>3.3700000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>92022</v>
@@ -616,44 +607,44 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3">
-        <v>7.3200000000000001E-4</v>
+        <v>4.3258427354548372E-2</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>7.3200000000000001E-4</v>
+        <v>4.3258427354548372E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
+        <v>92022</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2">
-        <v>92022</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="3">
-        <v>3.16E-3</v>
+        <v>9.6785567341690776E-3</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="3">
-        <v>3.16E-3</v>
+        <v>9.6785567341690776E-3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>92022</v>
@@ -662,21 +653,21 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3">
-        <v>7.2300000000000003E-3</v>
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.2261447283831553E-2</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
-        <v>7.2300000000000003E-3</v>
+      <c r="G10" s="2">
+        <v>6.2261447283831553E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
         <v>92022</v>
@@ -688,18 +679,18 @@
         <v>7</v>
       </c>
       <c r="E11" s="3">
-        <v>6.7900000000000002E-2</v>
+        <v>0.26067186033429762</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
       <c r="G11" s="3">
-        <v>6.7900000000000002E-2</v>
+        <v>0.26067186033429762</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>92022</v>
@@ -711,18 +702,18 @@
         <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.221</v>
+        <v>3.8537180167148827E-2</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>0.221</v>
+        <v>3.8537180167148827E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <v>92022</v>
@@ -734,18 +725,18 @@
         <v>9</v>
       </c>
       <c r="E13" s="3">
-        <v>5.1400000000000003E-4</v>
+        <v>0.29094685792349723</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <v>5.1400000000000003E-4</v>
+        <v>0.29094685792349723</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>92022</v>
@@ -757,18 +748,18 @@
         <v>10</v>
       </c>
       <c r="E14" s="3">
-        <v>1.8800000000000001E-2</v>
+        <v>3.9540445194471228E-3</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="3">
-        <v>1.8800000000000001E-2</v>
+        <v>3.9540445194471228E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>92022</v>
@@ -780,18 +771,18 @@
         <v>11</v>
       </c>
       <c r="E15" s="2">
-        <v>3.8100000000000002E-2</v>
+        <v>2.0950534394085498E-3</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>3.8100000000000002E-2</v>
+        <v>2.0950534394085498E-3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>92022</v>
@@ -802,83 +793,14 @@
       <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="3">
-        <v>4.62E-3</v>
+      <c r="E16" s="2">
+        <v>2.2986572243651561E-2</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="3">
-        <v>4.62E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2">
-        <v>92022</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3">
-        <v>9.5500000000000001E-4</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="3">
-        <v>9.5500000000000001E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="2">
-        <v>92022</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>4.3799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="2">
-        <v>92022</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.51220100000000002</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.51220100000000002</v>
+      <c r="G16" s="2">
+        <v>2.2986572243651561E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>